<commit_message>
removed password from ESF
</commit_message>
<xml_diff>
--- a/ESF/Univ_of_Southern_California-ESF-2023-10-25_0151-edit.xlsx
+++ b/ESF/Univ_of_Southern_California-ESF-2023-10-25_0151-edit.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" state="visible" r:id="rId3"/>
@@ -2248,7 +2248,7 @@
     <numFmt numFmtId="171" formatCode="0.0"/>
     <numFmt numFmtId="172" formatCode="0%"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2381,6 +2381,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Verdana"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Serif"/>
       <family val="0"/>
     </font>
   </fonts>
@@ -2687,7 +2693,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2695,19 +2701,19 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2747,23 +2753,23 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2771,7 +2777,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2779,19 +2785,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2807,7 +2813,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2815,7 +2821,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2823,11 +2829,11 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2843,11 +2849,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2855,7 +2861,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2863,23 +2869,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2887,15 +2893,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2915,15 +2921,15 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2935,7 +2941,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2943,11 +2949,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2983,7 +2989,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
@@ -2991,11 +2997,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3003,19 +3009,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3042,9 +3048,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3057,9 +3060,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3072,17 +3072,11 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
     </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3095,9 +3089,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3110,9 +3101,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3125,9 +3113,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3140,9 +3125,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3155,9 +3137,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3170,9 +3149,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3185,9 +3161,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3200,9 +3173,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3215,9 +3185,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3230,9 +3197,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3245,17 +3209,11 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
     </dxf>
     <dxf>
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3268,9 +3226,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3283,9 +3238,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3298,9 +3250,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3313,9 +3262,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3328,9 +3274,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3343,9 +3286,6 @@
       <font>
         <color rgb="FFFFFFFF"/>
       </font>
-      <fill>
-        <patternFill/>
-      </fill>
       <border diagonalUp="false" diagonalDown="false">
         <left/>
         <right/>
@@ -3621,11 +3561,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="52236430"/>
-        <c:axId val="40189536"/>
+        <c:axId val="91838761"/>
+        <c:axId val="42367824"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="52236430"/>
+        <c:axId val="91838761"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3702,12 +3642,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="40189536"/>
+        <c:crossAx val="42367824"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="40189536"/>
+        <c:axId val="42367824"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
@@ -3784,7 +3724,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="52236430"/>
+        <c:crossAx val="91838761"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4048,11 +3988,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="6583012"/>
-        <c:axId val="16639219"/>
+        <c:axId val="76856242"/>
+        <c:axId val="78286264"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="6583012"/>
+        <c:axId val="76856242"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4130,12 +4070,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="16639219"/>
+        <c:crossAx val="78286264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="16639219"/>
+        <c:axId val="78286264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4211,7 +4151,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6583012"/>
+        <c:crossAx val="76856242"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4268,15 +4208,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>124560</xdr:rowOff>
+      <xdr:colOff>132840</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>101880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>25560</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>883440</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>653760</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>178920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4289,8 +4229,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8400960" y="295920"/>
-          <a:ext cx="7695360" cy="3955680"/>
+          <a:off x="8541000" y="444960"/>
+          <a:ext cx="7499520" cy="3851280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4311,9 +4251,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>2160</xdr:colOff>
+      <xdr:colOff>1440</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>98640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4327,7 +4267,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="101520" y="272880"/>
-          <a:ext cx="7604640" cy="3001320"/>
+          <a:ext cx="7610040" cy="3000600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4348,14 +4288,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>72000</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>19080</xdr:rowOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>20880</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>125640</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>60480</xdr:rowOff>
+      <xdr:colOff>124920</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>63000</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -4363,8 +4303,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5078520" y="11624400"/>
-        <a:ext cx="4636800" cy="2887560"/>
+        <a:off x="5082840" y="11624400"/>
+        <a:ext cx="4638960" cy="2886840"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4378,14 +4318,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117360</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>173160</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>685080</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>66960</xdr:rowOff>
+      <xdr:colOff>684360</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4399,7 +4339,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="117360" y="5622840"/>
-          <a:ext cx="1962360" cy="1523160"/>
+          <a:ext cx="1962720" cy="1522440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4415,14 +4355,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>117360</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>154440</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>101160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>693360</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:colOff>692640</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>146520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4436,7 +4376,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="117360" y="7233480"/>
-          <a:ext cx="1970640" cy="1504080"/>
+          <a:ext cx="1971000" cy="1503360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4452,14 +4392,14 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>332280</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>41400</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>24840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>957240</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>350280</xdr:rowOff>
+      <xdr:colOff>956520</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>87840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4473,8 +4413,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2423880" y="5699160"/>
-          <a:ext cx="3539880" cy="2979720"/>
+          <a:off x="2426040" y="5699160"/>
+          <a:ext cx="3541320" cy="2979000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4490,14 +4430,14 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>380880</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>25920</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>180720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>126720</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>6120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -4506,8 +4446,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="1775520" y="6896520"/>
-          <a:ext cx="1140480" cy="867240"/>
+          <a:off x="1776600" y="6896520"/>
+          <a:ext cx="1141920" cy="867240"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4527,14 +4467,14 @@
     <xdr:from>
       <xdr:col>10</xdr:col>
       <xdr:colOff>6120</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>291960</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>54000</xdr:rowOff>
+      <xdr:colOff>291240</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>208080</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4547,8 +4487,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7504200" y="5803920"/>
-          <a:ext cx="3783600" cy="2578680"/>
+          <a:off x="7509240" y="5803920"/>
+          <a:ext cx="3785400" cy="2577960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4564,14 +4504,14 @@
     <xdr:from>
       <xdr:col>14</xdr:col>
       <xdr:colOff>29160</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>115920</xdr:rowOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>62640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>535680</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114120</xdr:rowOff>
+      <xdr:colOff>534960</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>60120</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4580,10 +4520,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="10327680" y="7194960"/>
-          <a:ext cx="1900800" cy="414720"/>
-          <a:chOff x="10327680" y="7194960"/>
-          <a:chExt cx="1900800" cy="414720"/>
+          <a:off x="10334520" y="7194960"/>
+          <a:ext cx="1901520" cy="414000"/>
+          <a:chOff x="10334520" y="7194960"/>
+          <a:chExt cx="1901520" cy="414000"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -4593,8 +4533,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="10985040" y="7356960"/>
-            <a:ext cx="1243440" cy="252720"/>
+            <a:off x="10992240" y="7356960"/>
+            <a:ext cx="1243800" cy="252000"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -4604,9 +4544,7 @@
           </a:solidFill>
           <a:ln w="9525">
             <a:solidFill>
-              <a:srgbClr val="ffffff">
-                <a:shade val="50000"/>
-              </a:srgbClr>
+              <a:srgbClr val="bcbcbc"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4649,8 +4587,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1" flipV="1">
-            <a:off x="10327680" y="7194960"/>
-            <a:ext cx="657360" cy="288720"/>
+            <a:off x="10334520" y="7194960"/>
+            <a:ext cx="658440" cy="289440"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -4671,14 +4609,14 @@
     <xdr:from>
       <xdr:col>18</xdr:col>
       <xdr:colOff>156240</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>146160</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>129600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>1064520</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>257400</xdr:rowOff>
+      <xdr:colOff>1063800</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>203400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4692,8 +4630,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13643640" y="5803920"/>
-          <a:ext cx="5788800" cy="2782080"/>
+          <a:off x="13651920" y="5803920"/>
+          <a:ext cx="5792760" cy="2781360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4709,14 +4647,14 @@
     <xdr:from>
       <xdr:col>19</xdr:col>
       <xdr:colOff>586080</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>91800</xdr:rowOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>165960</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>1080</xdr:rowOff>
+      <xdr:colOff>166680</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>156600</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
       <xdr:nvGrpSpPr>
@@ -4725,10 +4663,10 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="14770800" y="6337800"/>
-          <a:ext cx="1671480" cy="533880"/>
-          <a:chOff x="14770800" y="6337800"/>
-          <a:chExt cx="1671480" cy="533880"/>
+          <a:off x="14779440" y="6337800"/>
+          <a:ext cx="1674360" cy="534600"/>
+          <a:chOff x="14779440" y="6337800"/>
+          <a:chExt cx="1674360" cy="534600"/>
         </a:xfrm>
       </xdr:grpSpPr>
       <xdr:sp>
@@ -4738,8 +4676,8 @@
         </xdr:nvSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="14990400" y="6337800"/>
-            <a:ext cx="1053720" cy="277200"/>
+            <a:off x="14999400" y="6337800"/>
+            <a:ext cx="1054440" cy="276480"/>
           </a:xfrm>
           <a:prstGeom prst="rect">
             <a:avLst/>
@@ -4749,9 +4687,7 @@
           </a:solidFill>
           <a:ln w="9525">
             <a:solidFill>
-              <a:srgbClr val="ffffff">
-                <a:shade val="50000"/>
-              </a:srgbClr>
+              <a:srgbClr val="bcbcbc"/>
             </a:solidFill>
             <a:round/>
           </a:ln>
@@ -4794,8 +4730,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm flipH="1">
-            <a:off x="14770800" y="6479640"/>
-            <a:ext cx="219960" cy="379440"/>
+            <a:off x="14779440" y="6479640"/>
+            <a:ext cx="220680" cy="380160"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -4816,8 +4752,8 @@
         </xdr:nvCxnSpPr>
         <xdr:spPr>
           <a:xfrm>
-            <a:off x="16044480" y="6476400"/>
-            <a:ext cx="398160" cy="395640"/>
+            <a:off x="16054560" y="6476400"/>
+            <a:ext cx="399600" cy="396360"/>
           </a:xfrm>
           <a:prstGeom prst="straightConnector1">
             <a:avLst/>
@@ -4838,14 +4774,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>97560</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>105840</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>89280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>34</xdr:col>
-      <xdr:colOff>126360</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>11880</xdr:rowOff>
+      <xdr:colOff>125640</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>146880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4859,8 +4795,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20957400" y="5555520"/>
-          <a:ext cx="4212000" cy="3182400"/>
+          <a:off x="20970720" y="5555520"/>
+          <a:ext cx="4215240" cy="3181680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4876,14 +4812,14 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>234360</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>107640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>515880</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>30960</xdr:rowOff>
+      <xdr:colOff>515160</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>165960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4897,8 +4833,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27769320" y="5573880"/>
-          <a:ext cx="3767760" cy="3183120"/>
+          <a:off x="27786960" y="5573880"/>
+          <a:ext cx="3770280" cy="3182400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4914,14 +4850,14 @@
     <xdr:from>
       <xdr:col>46</xdr:col>
       <xdr:colOff>504000</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>100800</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>84240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>52</xdr:col>
-      <xdr:colOff>52920</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>7560</xdr:rowOff>
+      <xdr:colOff>52200</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>142560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -4935,8 +4871,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34714080" y="5550480"/>
-          <a:ext cx="3732120" cy="3183120"/>
+          <a:off x="34736040" y="5550480"/>
+          <a:ext cx="3735720" cy="3182400"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4952,14 +4888,14 @@
     <xdr:from>
       <xdr:col>45</xdr:col>
       <xdr:colOff>146520</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>65160</xdr:rowOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>48600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>46</xdr:col>
-      <xdr:colOff>344880</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>169920</xdr:rowOff>
+      <xdr:colOff>344160</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>115920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -4968,8 +4904,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="33659280" y="5722920"/>
-          <a:ext cx="895680" cy="693000"/>
+          <a:off x="33680880" y="5722920"/>
+          <a:ext cx="895320" cy="692280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4979,9 +4915,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -5033,14 +4967,14 @@
     <xdr:from>
       <xdr:col>46</xdr:col>
       <xdr:colOff>344880</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>203400</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>186840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>47</xdr:col>
       <xdr:colOff>693360</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>123480</xdr:rowOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>70200</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -5049,8 +4983,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="34554960" y="6069600"/>
-          <a:ext cx="1046160" cy="924840"/>
+          <a:off x="34576920" y="6069600"/>
+          <a:ext cx="1046880" cy="924840"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5070,14 +5004,14 @@
     <xdr:from>
       <xdr:col>36</xdr:col>
       <xdr:colOff>172080</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>195840</xdr:rowOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>179280</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>37</xdr:col>
-      <xdr:colOff>370440</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>92520</xdr:rowOff>
+      <xdr:colOff>369720</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5086,8 +5020,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27009720" y="5645520"/>
-          <a:ext cx="895680" cy="693000"/>
+          <a:off x="27027000" y="5645520"/>
+          <a:ext cx="895320" cy="692280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5097,9 +5031,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -5141,14 +5073,14 @@
     <xdr:from>
       <xdr:col>37</xdr:col>
       <xdr:colOff>370440</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>125640</xdr:rowOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>38</xdr:col>
       <xdr:colOff>361440</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>117000</xdr:rowOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>100440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -5157,8 +5089,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="27905400" y="5991840"/>
-          <a:ext cx="688680" cy="199800"/>
+          <a:off x="27923040" y="5991840"/>
+          <a:ext cx="689400" cy="199800"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5183,14 +5115,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>53280</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>10440</xdr:rowOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>165240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>46800</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>196920</xdr:rowOff>
+      <xdr:colOff>46080</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>160560</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5204,7 +5136,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="53280" y="6881040"/>
-          <a:ext cx="6280200" cy="2666880"/>
+          <a:ext cx="6284520" cy="2666160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5220,14 +5152,14 @@
     <xdr:from>
       <xdr:col>7</xdr:col>
       <xdr:colOff>228600</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>548640</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>190800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>116640</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>86400</xdr:rowOff>
+      <xdr:colOff>115920</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>32400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5240,8 +5172,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5120640" y="4027320"/>
-          <a:ext cx="2676960" cy="2721600"/>
+          <a:off x="5124600" y="4027320"/>
+          <a:ext cx="2678760" cy="2720880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5267,9 +5199,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>162360</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>28800</xdr:rowOff>
+      <xdr:colOff>161640</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>183240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5283,7 +5215,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="579240" y="1936800"/>
-          <a:ext cx="4463640" cy="3407040"/>
+          <a:ext cx="4467600" cy="3406320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5304,9 +5236,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>372240</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>51480</xdr:rowOff>
+      <xdr:colOff>371520</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>205920</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5319,8 +5251,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6366600" y="1600560"/>
-          <a:ext cx="5161320" cy="3765960"/>
+          <a:off x="6372360" y="1600560"/>
+          <a:ext cx="5164920" cy="3765240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5341,14 +5273,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>272160</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>5400</xdr:rowOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>53640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>576720</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>157320</xdr:rowOff>
+      <xdr:colOff>576000</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>128520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5362,7 +5294,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="272160" y="11476080"/>
-          <a:ext cx="7277040" cy="5159520"/>
+          <a:ext cx="7282440" cy="5158800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5379,13 +5311,13 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>337320</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>128520</xdr:rowOff>
+      <xdr:rowOff>150120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>326160</xdr:colOff>
-      <xdr:row>26</xdr:row>
-      <xdr:rowOff>182160</xdr:rowOff>
+      <xdr:colOff>325440</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>186480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5398,8 +5330,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9401400" y="1573920"/>
-          <a:ext cx="5566680" cy="4339800"/>
+          <a:off x="9409680" y="1573920"/>
+          <a:ext cx="5571000" cy="4339080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5415,14 +5347,14 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>239400</xdr:colOff>
-      <xdr:row>73</xdr:row>
-      <xdr:rowOff>224640</xdr:rowOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>196560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>94320</xdr:colOff>
-      <xdr:row>91</xdr:row>
-      <xdr:rowOff>113400</xdr:rowOff>
+      <xdr:colOff>93600</xdr:colOff>
+      <xdr:row>104</xdr:row>
+      <xdr:rowOff>78120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5436,7 +5368,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="239400" y="16702920"/>
-          <a:ext cx="8221680" cy="3790080"/>
+          <a:ext cx="8228520" cy="3789360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5453,13 +5385,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>83520</xdr:colOff>
       <xdr:row>10</xdr:row>
-      <xdr:rowOff>137880</xdr:rowOff>
+      <xdr:rowOff>159480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>2160</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>68400</xdr:rowOff>
+      <xdr:colOff>1440</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>36000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5473,7 +5405,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="83520" y="1926000"/>
-          <a:ext cx="7588080" cy="3457440"/>
+          <a:ext cx="7594560" cy="3456720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5489,14 +5421,14 @@
     <xdr:from>
       <xdr:col>12</xdr:col>
       <xdr:colOff>52200</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>59400</xdr:rowOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>27720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>693000</xdr:colOff>
-      <xdr:row>54</xdr:row>
-      <xdr:rowOff>101520</xdr:rowOff>
+      <xdr:colOff>692280</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>14400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5509,8 +5441,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8418960" y="8461800"/>
-          <a:ext cx="7613280" cy="3318480"/>
+          <a:off x="8426520" y="8461800"/>
+          <a:ext cx="7618680" cy="3317760"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5536,9 +5468,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>18720</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>645840</xdr:rowOff>
+      <xdr:colOff>18000</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>78480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -5547,7 +5479,7 @@
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="23040" y="1756440"/>
-        <a:ext cx="4179240" cy="2441520"/>
+        <a:ext cx="4182120" cy="2440800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -5567,13 +5499,13 @@
       <xdr:col>1</xdr:col>
       <xdr:colOff>45720</xdr:colOff>
       <xdr:row>8</xdr:row>
-      <xdr:rowOff>78480</xdr:rowOff>
+      <xdr:rowOff>100080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>227880</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>794160</xdr:rowOff>
+      <xdr:colOff>227160</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -5586,8 +5518,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="743040" y="1523880"/>
-          <a:ext cx="3668400" cy="2822400"/>
+          <a:off x="743760" y="1523880"/>
+          <a:ext cx="3670560" cy="2821680"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5604,13 +5536,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>251280</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>87480</xdr:rowOff>
+      <xdr:rowOff>109080</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>248040</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>24120</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp>
       <xdr:nvCxnSpPr>
@@ -5619,8 +5551,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="3040200" y="2292120"/>
-          <a:ext cx="1391760" cy="353520"/>
+          <a:off x="3042720" y="2292120"/>
+          <a:ext cx="1392840" cy="353520"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -5641,13 +5573,13 @@
       <xdr:col>6</xdr:col>
       <xdr:colOff>201600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>133560</xdr:rowOff>
+      <xdr:rowOff>155160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>109080</xdr:colOff>
+      <xdr:colOff>108360</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>21960</xdr:rowOff>
+      <xdr:rowOff>42840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -5656,8 +5588,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4385160" y="1750320"/>
-          <a:ext cx="1301760" cy="1101240"/>
+          <a:off x="4388760" y="1750320"/>
+          <a:ext cx="1302480" cy="1100520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5667,9 +5599,7 @@
         </a:solidFill>
         <a:ln w="9525">
           <a:solidFill>
-            <a:srgbClr val="ffffff">
-              <a:shade val="50000"/>
-            </a:srgbClr>
+            <a:srgbClr val="bcbcbc"/>
           </a:solidFill>
           <a:round/>
         </a:ln>
@@ -5893,10 +5823,10 @@
       <selection pane="topLeft" activeCell="P18" activeCellId="0" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.3"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="8.72"/>
   </cols>
   <sheetData>
@@ -6583,7 +6513,6 @@
       <c r="H42" s="18"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="/DEnUfb55kwpXk+nLVerY+zQZEwHq3aMtD26pc5hc++4mKWe8EoyGxPOMlNICAq2CBHphDpiggyrIg2YK/CzVg==" saltValue="1eC+GX5UrrGVrp1oiwgM6w==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="26">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J1:L1"/>
@@ -6629,13 +6558,13 @@
   </sheetPr>
   <dimension ref="A1:U104"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K75" activeCellId="0" sqref="K75"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="L65" activeCellId="0" sqref="L65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="1" width="15.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="11.86"/>
@@ -9648,7 +9577,6 @@
       <c r="S104" s="31"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="EtxnnnzQIFsME74aAl17lHffQ8Bg2lDxxGr+xq3pK64/V1zJt7dwFtvY+9hy2wXUMBCEnzKTs9UJZ/rvmLaT3A==" saltValue="nlSLKLTkv52WIGE7Zb0miw==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="199">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:C3"/>
@@ -9918,13 +9846,13 @@
   </sheetPr>
   <dimension ref="A1:AE54"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L37" activeCellId="0" sqref="L37"/>
+      <selection pane="bottomLeft" activeCell="X24" activeCellId="0" sqref="X24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="9.14"/>
@@ -10349,7 +10277,7 @@
       <c r="AD14" s="39"/>
       <c r="AE14" s="39"/>
     </row>
-    <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="38"/>
       <c r="B15" s="38"/>
       <c r="C15" s="38"/>
@@ -10380,7 +10308,7 @@
       <c r="AD15" s="39"/>
       <c r="AE15" s="39"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -10411,7 +10339,7 @@
       <c r="AD16" s="39"/>
       <c r="AE16" s="39"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -10442,7 +10370,7 @@
       <c r="AD17" s="39"/>
       <c r="AE17" s="39"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -10473,7 +10401,7 @@
       <c r="AD18" s="39"/>
       <c r="AE18" s="39"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -10504,7 +10432,7 @@
       <c r="AD19" s="39"/>
       <c r="AE19" s="39"/>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -10535,7 +10463,7 @@
       <c r="AD20" s="39"/>
       <c r="AE20" s="39"/>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="38"/>
       <c r="B21" s="38"/>
       <c r="C21" s="38"/>
@@ -11218,7 +11146,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="46" t="s">
         <v>217</v>
       </c>
@@ -11541,7 +11469,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="KnKrFL5MkH14H4PyndxcrIH7RazjyhkF821IZ6ctT5tScsPLiAGtC4c3zonRo/wxCCjC5p7i74UUJaiACMcwIg==" saltValue="J8596+ZNEeq3f/NzixaZZQ==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="79">
     <mergeCell ref="A2:K27"/>
     <mergeCell ref="M2:W27"/>
@@ -11642,15 +11569,12 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="2" id="{657E3F4A-B81D-4281-A132-334F607433AB}">
+          <x14:cfRule type="expression" priority="2" id="{6BD05064-DD75-4241-949C-ACCB706A2814}">
             <xm:f>Accumulator!$D$62 = "Team Designed"</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FFFFFFFF"/>
               </font>
-              <fill>
-                <patternFill/>
-              </fill>
               <border diagonalUp="false" diagonalDown="false">
                 <left/>
                 <right/>
@@ -11663,15 +11587,12 @@
           <xm:sqref>K30:K43 K48:K54</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="3" id="{E6601D1F-594E-40D7-B268-F08D80B95490}">
+          <x14:cfRule type="expression" priority="3" id="{251B8A80-1611-41DB-A992-C7B7A084BBA3}">
             <xm:f>Accumulator!$D$62 = "Team Designed"</xm:f>
             <x14:dxf>
               <font>
                 <color rgb="FFFFFFFF"/>
               </font>
-              <fill>
-                <patternFill/>
-              </fill>
               <border diagonalUp="false" diagonalDown="false">
                 <left/>
                 <right/>
@@ -11702,7 +11623,7 @@
       <selection pane="bottomLeft" activeCell="O18" activeCellId="0" sqref="O18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.29"/>
@@ -12376,7 +12297,7 @@
       <c r="AJ15" s="11"/>
       <c r="AK15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>5</v>
       </c>
@@ -12451,7 +12372,7 @@
       <c r="AJ16" s="11"/>
       <c r="AK16" s="11"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>6</v>
       </c>
@@ -12538,7 +12459,7 @@
       <c r="AJ17" s="11"/>
       <c r="AK17" s="11"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>7</v>
       </c>
@@ -12597,7 +12518,7 @@
       <c r="AJ18" s="11"/>
       <c r="AK18" s="11"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>8</v>
       </c>
@@ -12662,7 +12583,7 @@
       <c r="AJ19" s="11"/>
       <c r="AK19" s="11"/>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>9</v>
       </c>
@@ -13503,7 +13424,7 @@
       <c r="AZ39" s="38"/>
       <c r="BA39" s="38"/>
     </row>
-    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="38"/>
       <c r="B40" s="38"/>
       <c r="C40" s="38"/>
@@ -14680,7 +14601,7 @@
       <c r="G63" s="31"/>
       <c r="H63" s="31"/>
     </row>
-    <row r="64" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="22" t="s">
         <v>333</v>
       </c>
@@ -14742,7 +14663,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="22" t="s">
         <v>336</v>
       </c>
@@ -14765,7 +14686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="22" t="s">
         <v>337</v>
       </c>
@@ -14788,7 +14709,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="22" t="s">
         <v>338</v>
       </c>
@@ -14803,12 +14724,12 @@
         <v/>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="1" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="74" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="51" t="s">
         <v>340</v>
@@ -14933,7 +14854,6 @@
       <c r="C90" s="29"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="5G0AmqaoDrsIRuy5+I3R/L2IZTkzNtWi6TI3gjFgF23irMptfaaqq0HUvxAkprKqKmEVLraT5Rwbd9jNbOdcOw==" saltValue="eyHSNWMo9+kDPUMtBH3J0w==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="170">
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="A4:D4"/>
@@ -15249,7 +15169,7 @@
       <selection pane="topLeft" activeCell="M19" activeCellId="0" sqref="M19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="1" style="1" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="8.86"/>
@@ -15775,7 +15695,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="22" t="s">
         <v>377</v>
       </c>
@@ -15802,7 +15722,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="22" t="s">
         <v>388</v>
       </c>
@@ -15820,7 +15740,7 @@
       </c>
       <c r="H17" s="62"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="65" t="s">
         <v>389</v>
       </c>
@@ -15838,7 +15758,7 @@
       </c>
       <c r="H18" s="66"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="22" t="s">
         <v>391</v>
       </c>
@@ -15852,7 +15772,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="22" t="s">
         <v>383</v>
       </c>
@@ -16052,7 +15972,7 @@
       <c r="F39" s="68"/>
       <c r="G39" s="68"/>
     </row>
-    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="68"/>
       <c r="B40" s="68"/>
       <c r="C40" s="68"/>
@@ -16077,7 +15997,6 @@
     <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="Uie6Up9mZNuuOviMksw684vE7s2Tx9rN8euwciuXDm6BEptKmEKT2718jjHXkQWjacPi1WWG+8sEBdw4GXCp3A==" saltValue="caFEWMACSrtFVdwIMA4kog==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="56">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>
@@ -16194,7 +16113,7 @@
       <selection pane="bottomLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="8.72"/>
   </cols>
@@ -16490,7 +16409,7 @@
       <c r="P15" s="38"/>
       <c r="Q15" s="38"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -16508,7 +16427,7 @@
       <c r="P16" s="38"/>
       <c r="Q16" s="38"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -16526,7 +16445,7 @@
       <c r="P17" s="38"/>
       <c r="Q17" s="38"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -16544,7 +16463,7 @@
       <c r="P18" s="38"/>
       <c r="Q18" s="38"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -16562,7 +16481,7 @@
       <c r="P19" s="38"/>
       <c r="Q19" s="38"/>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -17043,7 +16962,7 @@
         <v>BLANK</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="2" t="s">
         <v>20</v>
       </c>
@@ -17128,7 +17047,6 @@
       <c r="P44" s="11"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="8UGjOur+APRSAGtBeGORuUB3xwSQHK/gTiN2NaaGNoJCBiNOH2celYgsgqnApKlO/FLGpHugjSW4GOdw/hBo+w==" saltValue="x2xWcABdJS46AOCyrtn/gw==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="52">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="H2:N2"/>
@@ -17219,7 +17137,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:W95"/>
+  <dimension ref="A1:W103"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A45" activePane="bottomLeft" state="frozen"/>
@@ -17227,12 +17145,12 @@
       <selection pane="bottomLeft" activeCell="X70" activeCellId="0" sqref="X70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -17241,7 +17159,7 @@
         <v>WARNING</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
@@ -17265,7 +17183,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="70" t="s">
         <v>424</v>
       </c>
@@ -17287,7 +17205,7 @@
       <c r="L3" s="71"/>
       <c r="M3" s="48"/>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>269</v>
       </c>
@@ -17544,7 +17462,7 @@
       <c r="V15" s="38"/>
       <c r="W15" s="38"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="38"/>
       <c r="B16" s="38"/>
       <c r="C16" s="38"/>
@@ -17568,7 +17486,7 @@
       <c r="V16" s="38"/>
       <c r="W16" s="38"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="38"/>
       <c r="B17" s="38"/>
       <c r="C17" s="38"/>
@@ -17592,7 +17510,7 @@
       <c r="V17" s="38"/>
       <c r="W17" s="38"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="38"/>
       <c r="B18" s="38"/>
       <c r="C18" s="38"/>
@@ -17616,7 +17534,7 @@
       <c r="V18" s="38"/>
       <c r="W18" s="38"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="38"/>
       <c r="B19" s="38"/>
       <c r="C19" s="38"/>
@@ -17640,7 +17558,7 @@
       <c r="V19" s="38"/>
       <c r="W19" s="38"/>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="38"/>
       <c r="B20" s="38"/>
       <c r="C20" s="38"/>
@@ -18168,7 +18086,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="46" t="s">
         <v>445</v>
       </c>
@@ -18677,7 +18595,7 @@
       <c r="V54" s="38"/>
       <c r="W54" s="38"/>
     </row>
-    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="46" t="s">
         <v>463</v>
       </c>
@@ -18711,7 +18629,7 @@
       <c r="V55" s="38"/>
       <c r="W55" s="38"/>
     </row>
-    <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="46"/>
       <c r="B56" s="46"/>
       <c r="C56" s="22" t="s">
@@ -18743,7 +18661,7 @@
       <c r="V56" s="38"/>
       <c r="W56" s="38"/>
     </row>
-    <row r="57" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="46" t="s">
         <v>468</v>
       </c>
@@ -18965,7 +18883,7 @@
       <c r="V63" s="38"/>
       <c r="W63" s="38"/>
     </row>
-    <row r="64" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="76"/>
       <c r="B64" s="76"/>
       <c r="C64" s="76"/>
@@ -19063,7 +18981,7 @@
       <c r="V68" s="38"/>
       <c r="W68" s="38"/>
     </row>
-    <row r="69" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M69" s="38"/>
       <c r="N69" s="38"/>
       <c r="O69" s="38"/>
@@ -19076,7 +18994,7 @@
       <c r="V69" s="38"/>
       <c r="W69" s="38"/>
     </row>
-    <row r="70" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M70" s="38"/>
       <c r="N70" s="38"/>
       <c r="O70" s="38"/>
@@ -19089,7 +19007,7 @@
       <c r="V70" s="38"/>
       <c r="W70" s="38"/>
     </row>
-    <row r="71" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M71" s="38"/>
       <c r="N71" s="38"/>
       <c r="O71" s="38"/>
@@ -19102,7 +19020,7 @@
       <c r="V71" s="38"/>
       <c r="W71" s="38"/>
     </row>
-    <row r="72" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M72" s="38"/>
       <c r="N72" s="38"/>
       <c r="O72" s="38"/>
@@ -19115,7 +19033,7 @@
       <c r="V72" s="38"/>
       <c r="W72" s="38"/>
     </row>
-    <row r="73" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="M73" s="38"/>
       <c r="N73" s="38"/>
       <c r="O73" s="38"/>
@@ -19290,10 +19208,20 @@
     <row r="88" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="89" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="91" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="92" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="93" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="95" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="96" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="97" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="98" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="99" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="100" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="101" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="102" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="103" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="uZxEkseIZLvN/jjfBo9LYLbmQEjt+RVf+OR7BSB9yn4Zkoi82i7jJJKSn6xkZFv/YsH2JZVBaO9fx0+3hNFzLg==" saltValue="c/G76iUMjFLEHM4nPLuwwQ==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="93">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:F3"/>
@@ -19427,7 +19355,7 @@
       <selection pane="bottomLeft" activeCell="M13" activeCellId="0" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="1" style="1" width="8.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="12.57"/>
@@ -19846,8 +19774,11 @@
     <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -19857,7 +19788,6 @@
       <c r="A28" s="80"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="SFIIq+U30TtKj2sHy/FKJjnBzCoQLzjV1mMwtMATDsej8y5ACEmaOxv4GFSmAOG6dozeC5NoalaD4ESnz0bTvg==" saltValue="ZCaZhKBTuCR0NTkj/h6/xQ==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="48">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="F2:F3"/>
@@ -19937,12 +19867,12 @@
       <selection pane="topLeft" activeCell="K30" activeCellId="0" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="13.5" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="1" width="8.72"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="19" t="s">
         <v>1</v>
       </c>
@@ -19951,7 +19881,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
         <v>220</v>
       </c>
@@ -19975,7 +19905,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
         <v>30</v>
       </c>
@@ -20003,7 +19933,7 @@
         <v>OK</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="20" t="s">
         <v>32</v>
       </c>
@@ -20156,7 +20086,7 @@
       <c r="G15" s="84"/>
       <c r="H15" s="84"/>
     </row>
-    <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="84"/>
       <c r="B16" s="84"/>
       <c r="C16" s="84"/>
@@ -20166,7 +20096,7 @@
       <c r="G16" s="84"/>
       <c r="H16" s="84"/>
     </row>
-    <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="84"/>
       <c r="B17" s="84"/>
       <c r="C17" s="84"/>
@@ -20176,7 +20106,7 @@
       <c r="G17" s="84"/>
       <c r="H17" s="84"/>
     </row>
-    <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="84"/>
       <c r="B18" s="84"/>
       <c r="C18" s="84"/>
@@ -20186,7 +20116,7 @@
       <c r="G18" s="84"/>
       <c r="H18" s="84"/>
     </row>
-    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="84"/>
       <c r="B19" s="84"/>
       <c r="C19" s="84"/>
@@ -20196,7 +20126,7 @@
       <c r="G19" s="84"/>
       <c r="H19" s="84"/>
     </row>
-    <row r="20" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="84"/>
       <c r="B20" s="84"/>
       <c r="C20" s="84"/>
@@ -20357,7 +20287,6 @@
       <c r="G34" s="74"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="EFUYjzGyJAN41JDq0Vx4FhQgnnpCR/UREV+o2MTohhkIa9XZbW1nOBqgLqW/i0bVb2JPNzBSWas6c1lQJaYmAw==" saltValue="Wj3kCR1k+cUSscRm0QRxNA==" spinCount="100000" sheet="true" scenarios="true" insertHyperlinks="false"/>
   <mergeCells count="23">
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="G2:K2"/>

</xml_diff>